<commit_message>
Docs: [Documentação] Burndown Atualizado
</commit_message>
<xml_diff>
--- a/Docs/docs_tecnicos/Burndown codenine.xlsx
+++ b/Docs/docs_tecnicos/Burndown codenine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmaci\OneDrive\Área de Trabalho\portfolio_digital_dsm\API-2024.1\Docs\docs_tecnicos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmaci\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39F88EA-C20A-42AE-A570-DABBB5D91A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11C4AF5-3F31-41A9-8AC9-9D1AE5893CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
   <si>
     <t>Data de início:</t>
   </si>
@@ -127,6 +127,78 @@
   <si>
     <t>Davi</t>
   </si>
+  <si>
+    <t>Criação da barra de navegação</t>
+  </si>
+  <si>
+    <t>Desenvolvimento do Banco de Dados Físico</t>
+  </si>
+  <si>
+    <t>Eduardo</t>
+  </si>
+  <si>
+    <t>Desenvolvimento do Sprint Backlog</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da tela de cadastro do cliente</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da tela de cadastro do funcionário</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da tela de login do cliente</t>
+  </si>
+  <si>
+    <t>Jonas</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da tela de login do funcionário</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da tela de edição de dados do cliente</t>
+  </si>
+  <si>
+    <t>Yuri</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da tela de edição de dados do funcionário</t>
+  </si>
+  <si>
+    <t>Sistema de Cadastro</t>
+  </si>
+  <si>
+    <t>Sistema de Login</t>
+  </si>
+  <si>
+    <t>Davi e Joyce</t>
+  </si>
+  <si>
+    <t>Sistema de edição de dados</t>
+  </si>
+  <si>
+    <t>Davi, Joyce e Yuri</t>
+  </si>
+  <si>
+    <t>Sistema de visualização de usuários</t>
+  </si>
+  <si>
+    <t>Yuri e Joyce</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da tela de FAQ</t>
+  </si>
+  <si>
+    <t>Estudo de TypeOrm</t>
+  </si>
+  <si>
+    <t>Joyce</t>
+  </si>
+  <si>
+    <t>Documentação do projeto no Git</t>
+  </si>
 </sst>
 </file>
 
@@ -136,7 +208,7 @@
     <numFmt numFmtId="164" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -173,6 +245,18 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -333,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -395,12 +479,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -410,14 +503,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,10 +904,10 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1161,64 +1249,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>109.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>103.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>97.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>86.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>80.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>74.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>63.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>57.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>51.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>40.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>28.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>17.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>5.75</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1325,64 +1413,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -3055,8 +3143,8 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3076,7 +3164,7 @@
       </c>
       <c r="E1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45392</v>
+        <v>45417</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3482,7 +3570,7 @@
       </c>
       <c r="E22" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3503,7 +3591,7 @@
       </c>
       <c r="E23" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3552,30 +3640,30 @@
       <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="49"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="38"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="35"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="6" t="s">
         <v>10</v>
       </c>
@@ -3591,15 +3679,15 @@
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
       <c r="H29" s="10">
         <v>45380</v>
       </c>
@@ -3616,15 +3704,15 @@
       <c r="N29" s="9"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="41"/>
       <c r="H30" s="10">
         <v>45376</v>
       </c>
@@ -3641,15 +3729,15 @@
       <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="35"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="41"/>
       <c r="H31" s="13">
         <v>45381</v>
       </c>
@@ -3665,15 +3753,15 @@
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="41"/>
       <c r="H32" s="10">
         <v>45384</v>
       </c>
@@ -3689,15 +3777,15 @@
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="42"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="47"/>
       <c r="H33" s="10">
         <v>45378</v>
       </c>
@@ -3713,15 +3801,15 @@
       <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="42"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="47"/>
       <c r="H34" s="14">
         <v>45385</v>
       </c>
@@ -3737,15 +3825,15 @@
       <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="42"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="47"/>
       <c r="H35" s="14">
         <v>45388</v>
       </c>
@@ -3761,15 +3849,15 @@
       <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="42"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="47"/>
       <c r="H36" s="14">
         <v>45388</v>
       </c>
@@ -5187,8 +5275,8 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5208,7 +5296,7 @@
       </c>
       <c r="E1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45392</v>
+        <v>45417</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5249,7 +5337,7 @@
       </c>
       <c r="C5" s="7">
         <f>SUM(J29:J1007)</f>
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" ref="D5:D25" si="0">SUMIF($K$29:$K$1007,B5,$J$29:$J$1007)</f>
@@ -5257,7 +5345,7 @@
       </c>
       <c r="E5" s="7">
         <f>C5-D5</f>
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5270,7 +5358,7 @@
       </c>
       <c r="C6" s="7">
         <f t="shared" ref="C6:C25" si="2">C5-$C$5/($B$2-1)</f>
-        <v>0</v>
+        <v>109.25</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
@@ -5278,7 +5366,7 @@
       </c>
       <c r="E6" s="7">
         <f t="shared" ref="E6:E25" ca="1" si="3">IF(B6&lt;=$E$1,E5-D6,)</f>
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5291,15 +5379,15 @@
       </c>
       <c r="C7" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>103.5</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5312,15 +5400,15 @@
       </c>
       <c r="C8" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>97.75</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5333,15 +5421,15 @@
       </c>
       <c r="C9" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5354,7 +5442,7 @@
       </c>
       <c r="C10" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>86.25</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
@@ -5362,7 +5450,7 @@
       </c>
       <c r="E10" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5375,7 +5463,7 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>80.5</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" si="0"/>
@@ -5383,7 +5471,7 @@
       </c>
       <c r="E11" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5396,15 +5484,15 @@
       </c>
       <c r="C12" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>74.75</v>
       </c>
       <c r="D12" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5417,7 +5505,7 @@
       </c>
       <c r="C13" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D13" s="7">
         <f t="shared" si="0"/>
@@ -5425,7 +5513,7 @@
       </c>
       <c r="E13" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5438,7 +5526,7 @@
       </c>
       <c r="C14" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>63.25</v>
       </c>
       <c r="D14" s="7">
         <f t="shared" si="0"/>
@@ -5446,7 +5534,7 @@
       </c>
       <c r="E14" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5459,7 +5547,7 @@
       </c>
       <c r="C15" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>57.5</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" si="0"/>
@@ -5467,7 +5555,7 @@
       </c>
       <c r="E15" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5480,15 +5568,15 @@
       </c>
       <c r="C16" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>51.75</v>
       </c>
       <c r="D16" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5501,15 +5589,15 @@
       </c>
       <c r="C17" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D17" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5522,15 +5610,15 @@
       </c>
       <c r="C18" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40.25</v>
       </c>
       <c r="D18" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E18" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5543,15 +5631,15 @@
       </c>
       <c r="C19" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>34.5</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5564,7 +5652,7 @@
       </c>
       <c r="C20" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28.75</v>
       </c>
       <c r="D20" s="7">
         <f t="shared" si="0"/>
@@ -5572,7 +5660,7 @@
       </c>
       <c r="E20" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5585,15 +5673,15 @@
       </c>
       <c r="C21" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D21" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E21" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5606,15 +5694,15 @@
       </c>
       <c r="C22" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17.25</v>
       </c>
       <c r="D22" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E22" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5627,15 +5715,15 @@
       </c>
       <c r="C23" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="D23" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5648,15 +5736,15 @@
       </c>
       <c r="C24" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.75</v>
       </c>
       <c r="D24" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5673,7 +5761,7 @@
       </c>
       <c r="D25" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E25" s="7">
         <f t="shared" ca="1" si="3"/>
@@ -5684,30 +5772,30 @@
       <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="35"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="41"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="35"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="6" t="s">
         <v>10</v>
       </c>
@@ -5723,239 +5811,399 @@
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="12"/>
+      <c r="A29" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="10">
+        <v>45397</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="16">
+        <v>10</v>
+      </c>
+      <c r="K29" s="12">
+        <v>45401</v>
+      </c>
       <c r="L29" s="5"/>
       <c r="N29" s="9"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="39"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="12"/>
+      <c r="A30" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="10">
+        <v>45398</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30" s="17">
+        <v>3</v>
+      </c>
+      <c r="K30" s="12">
+        <v>45400</v>
+      </c>
       <c r="L30" s="5"/>
       <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="39"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="12"/>
+      <c r="A31" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="13">
+        <v>45405</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J31" s="18">
+        <v>4</v>
+      </c>
+      <c r="K31" s="12">
+        <v>45413</v>
+      </c>
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="39"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="12"/>
+      <c r="A32" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="10">
+        <v>45406</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" s="11">
+        <v>5</v>
+      </c>
+      <c r="K32" s="12">
+        <v>45414</v>
+      </c>
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="40"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="12"/>
+      <c r="A33" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="10">
+        <v>45401</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J33" s="11">
+        <v>4</v>
+      </c>
+      <c r="K33" s="12">
+        <v>45408</v>
+      </c>
       <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="12"/>
+      <c r="A34" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="14">
+        <v>45402</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J34" s="7">
+        <v>4</v>
+      </c>
+      <c r="K34" s="12">
+        <v>45409</v>
+      </c>
       <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="40"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="12"/>
+      <c r="A35" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="14">
+        <v>45402</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35" s="15">
+        <v>5</v>
+      </c>
+      <c r="K35" s="12">
+        <v>45410</v>
+      </c>
       <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="39"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="12"/>
+      <c r="A36" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="14">
+        <v>45402</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J36" s="7">
+        <v>6</v>
+      </c>
+      <c r="K36" s="12">
+        <v>45410</v>
+      </c>
       <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="43"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="8"/>
+      <c r="A37" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="8">
+        <v>45399</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="7">
+        <v>13</v>
+      </c>
+      <c r="K37" s="8">
+        <v>45404</v>
+      </c>
       <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="39"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="8"/>
+      <c r="A38" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="8">
+        <v>45410</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J38" s="7">
+        <v>18</v>
+      </c>
+      <c r="K38" s="8">
+        <v>45415</v>
+      </c>
       <c r="L38" s="5"/>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="39"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="8"/>
+      <c r="A39" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="8">
+        <v>45411</v>
+      </c>
+      <c r="I39" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="J39" s="7">
+        <v>15</v>
+      </c>
+      <c r="K39" s="8">
+        <v>45416</v>
+      </c>
       <c r="L39" s="5"/>
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="39"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="8"/>
+      <c r="A40" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="8">
+        <v>45411</v>
+      </c>
+      <c r="I40" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="J40" s="7">
+        <v>9</v>
+      </c>
+      <c r="K40" s="8">
+        <v>45415</v>
+      </c>
       <c r="L40" s="5"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="46"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="19"/>
+      <c r="A41" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="19">
+        <v>45407</v>
+      </c>
+      <c r="I41" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="J41" s="21">
+        <v>8</v>
+      </c>
+      <c r="K41" s="19">
+        <v>45411</v>
+      </c>
       <c r="L41" s="5"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="39"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="8"/>
+      <c r="A42" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="8">
+        <v>45398</v>
+      </c>
+      <c r="I42" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="J42" s="7">
+        <v>5</v>
+      </c>
+      <c r="K42" s="8">
+        <v>45401</v>
+      </c>
       <c r="L42" s="5"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="39"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="8"/>
+      <c r="A43" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="8">
+        <v>45397</v>
+      </c>
+      <c r="I43" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J43" s="7">
+        <v>3</v>
+      </c>
+      <c r="K43" s="8">
+        <v>45399</v>
+      </c>
       <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="39"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="8"/>
+      <c r="A44" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="8">
+        <v>45415</v>
+      </c>
+      <c r="I44" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J44" s="7">
+        <v>3</v>
+      </c>
+      <c r="K44" s="8">
+        <v>45417</v>
+      </c>
       <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="39"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="35"/>
+      <c r="A45" s="44"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="41"/>
       <c r="H45" s="8"/>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
@@ -5963,13 +6211,13 @@
       <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="39"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="35"/>
+      <c r="A46" s="44"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="41"/>
       <c r="H46" s="8"/>
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
@@ -5977,13 +6225,13 @@
       <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="39"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="35"/>
+      <c r="A47" s="44"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="41"/>
       <c r="H47" s="8"/>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
@@ -5991,13 +6239,13 @@
       <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="39"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="35"/>
+      <c r="A48" s="44"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="41"/>
       <c r="H48" s="8"/>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
@@ -6005,13 +6253,13 @@
       <c r="L48" s="5"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="39"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="35"/>
+      <c r="A49" s="44"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="41"/>
       <c r="H49" s="8"/>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
@@ -6019,13 +6267,13 @@
       <c r="L49" s="5"/>
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="39"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="35"/>
+      <c r="A50" s="44"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="41"/>
       <c r="H50" s="8"/>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
@@ -6033,13 +6281,13 @@
       <c r="L50" s="5"/>
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="39"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="35"/>
+      <c r="A51" s="44"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="41"/>
       <c r="H51" s="8"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
@@ -6047,13 +6295,13 @@
       <c r="L51" s="5"/>
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="39"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="35"/>
+      <c r="A52" s="44"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="41"/>
       <c r="H52" s="8"/>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
@@ -6061,13 +6309,13 @@
       <c r="L52" s="5"/>
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="39"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="35"/>
+      <c r="A53" s="44"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="41"/>
       <c r="H53" s="8"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
@@ -6075,13 +6323,13 @@
       <c r="L53" s="5"/>
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="39"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="35"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="41"/>
       <c r="H54" s="8"/>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
@@ -6089,13 +6337,13 @@
       <c r="L54" s="5"/>
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="39"/>
-      <c r="B55" s="34"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="35"/>
+      <c r="A55" s="44"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="41"/>
       <c r="H55" s="8"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
@@ -6103,13 +6351,13 @@
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="39"/>
-      <c r="B56" s="34"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="35"/>
+      <c r="A56" s="44"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="41"/>
       <c r="H56" s="8"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
@@ -6117,13 +6365,13 @@
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="39"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="35"/>
+      <c r="A57" s="44"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="41"/>
       <c r="H57" s="8"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
@@ -6131,13 +6379,13 @@
       <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="39"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="35"/>
+      <c r="A58" s="44"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="41"/>
       <c r="H58" s="8"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
@@ -6145,13 +6393,13 @@
       <c r="L58" s="5"/>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="39"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="35"/>
+      <c r="A59" s="44"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="41"/>
       <c r="H59" s="8"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
@@ -6159,13 +6407,13 @@
       <c r="L59" s="5"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="39"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="35"/>
+      <c r="A60" s="44"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="41"/>
       <c r="H60" s="8"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
@@ -6173,13 +6421,13 @@
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="39"/>
-      <c r="B61" s="34"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="35"/>
+      <c r="A61" s="44"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="41"/>
       <c r="H61" s="8"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
@@ -6187,13 +6435,13 @@
       <c r="L61" s="5"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="39"/>
-      <c r="B62" s="34"/>
-      <c r="C62" s="34"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="35"/>
+      <c r="A62" s="44"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="41"/>
       <c r="H62" s="8"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
@@ -6201,13 +6449,13 @@
       <c r="L62" s="5"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="39"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="35"/>
+      <c r="A63" s="44"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="41"/>
       <c r="H63" s="8"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
@@ -6215,13 +6463,13 @@
       <c r="L63" s="5"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="39"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="35"/>
+      <c r="A64" s="44"/>
+      <c r="B64" s="40"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="41"/>
       <c r="H64" s="8"/>
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
@@ -6229,13 +6477,13 @@
       <c r="L64" s="5"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="39"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="35"/>
+      <c r="A65" s="44"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="41"/>
       <c r="H65" s="8"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
@@ -6243,13 +6491,13 @@
       <c r="L65" s="5"/>
     </row>
     <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="39"/>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="35"/>
+      <c r="A66" s="44"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="41"/>
       <c r="H66" s="8"/>
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
@@ -6257,13 +6505,13 @@
       <c r="L66" s="5"/>
     </row>
     <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="39"/>
-      <c r="B67" s="34"/>
-      <c r="C67" s="34"/>
-      <c r="D67" s="34"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="35"/>
+      <c r="A67" s="44"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="40"/>
+      <c r="G67" s="41"/>
       <c r="H67" s="8"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
@@ -9535,7 +9783,7 @@
       </c>
       <c r="E1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45392</v>
+        <v>45417</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10011,30 +10259,30 @@
       <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="35"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="41"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="35"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="6" t="s">
         <v>10</v>
       </c>
@@ -10050,13 +10298,13 @@
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
       <c r="H29" s="22"/>
       <c r="I29" s="7"/>
       <c r="J29" s="23"/>
@@ -10065,13 +10313,13 @@
       <c r="N29" s="9"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="39"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
+      <c r="A30" s="44"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="41"/>
       <c r="H30" s="22"/>
       <c r="I30" s="7"/>
       <c r="J30" s="11"/>
@@ -10080,13 +10328,13 @@
       <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="39"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="35"/>
+      <c r="A31" s="44"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="41"/>
       <c r="H31" s="22"/>
       <c r="I31" s="7"/>
       <c r="J31" s="11"/>
@@ -10094,13 +10342,13 @@
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="39"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
+      <c r="A32" s="44"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="41"/>
       <c r="H32" s="22"/>
       <c r="I32" s="7"/>
       <c r="J32" s="23"/>
@@ -10108,13 +10356,13 @@
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="46"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="41"/>
       <c r="H33" s="24"/>
       <c r="I33" s="20"/>
       <c r="J33" s="25"/>
@@ -10122,13 +10370,13 @@
       <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="47"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="45"/>
+      <c r="A34" s="53"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="50"/>
       <c r="H34" s="27"/>
       <c r="I34" s="28"/>
       <c r="J34" s="23"/>
@@ -10136,13 +10384,13 @@
       <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="47"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="45"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="50"/>
       <c r="H35" s="27"/>
       <c r="I35" s="28"/>
       <c r="J35" s="30"/>
@@ -10150,13 +10398,13 @@
       <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="47"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="45"/>
+      <c r="A36" s="53"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="50"/>
       <c r="H36" s="27"/>
       <c r="I36" s="28"/>
       <c r="J36" s="30"/>
@@ -10164,13 +10412,13 @@
       <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="47"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="45"/>
+      <c r="A37" s="53"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="50"/>
       <c r="H37" s="27"/>
       <c r="I37" s="28"/>
       <c r="J37" s="23"/>
@@ -10178,13 +10426,13 @@
       <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="47"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="45"/>
+      <c r="A38" s="53"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="50"/>
       <c r="H38" s="27"/>
       <c r="I38" s="28"/>
       <c r="J38" s="23"/>
@@ -10192,13 +10440,13 @@
       <c r="L38" s="5"/>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="47"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="45"/>
+      <c r="A39" s="53"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="50"/>
       <c r="H39" s="27"/>
       <c r="I39" s="28"/>
       <c r="J39" s="30"/>
@@ -10206,13 +10454,13 @@
       <c r="L39" s="5"/>
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="47"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="45"/>
+      <c r="A40" s="53"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="50"/>
       <c r="H40" s="27"/>
       <c r="I40" s="28"/>
       <c r="J40" s="30"/>
@@ -10220,13 +10468,13 @@
       <c r="L40" s="5"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="47"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="45"/>
+      <c r="A41" s="53"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="50"/>
       <c r="H41" s="27"/>
       <c r="I41" s="28"/>
       <c r="J41" s="30"/>
@@ -10234,13 +10482,13 @@
       <c r="L41" s="5"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="47"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="45"/>
+      <c r="A42" s="53"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="50"/>
       <c r="H42" s="27"/>
       <c r="I42" s="28"/>
       <c r="J42" s="30"/>
@@ -10248,13 +10496,13 @@
       <c r="L42" s="5"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="47"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="45"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="50"/>
       <c r="H43" s="31"/>
       <c r="I43" s="28"/>
       <c r="J43" s="28"/>
@@ -10262,13 +10510,13 @@
       <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="47"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="50"/>
       <c r="H44" s="27"/>
       <c r="I44" s="28"/>
       <c r="J44" s="28"/>
@@ -10276,13 +10524,13 @@
       <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="39"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="35"/>
+      <c r="A45" s="44"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="41"/>
       <c r="H45" s="22"/>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
@@ -10290,13 +10538,13 @@
       <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="39"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="35"/>
+      <c r="A46" s="44"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="41"/>
       <c r="H46" s="8"/>
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
@@ -10304,13 +10552,13 @@
       <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="39"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="35"/>
+      <c r="A47" s="44"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="41"/>
       <c r="H47" s="8"/>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
@@ -10318,13 +10566,13 @@
       <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="39"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="35"/>
+      <c r="A48" s="44"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="41"/>
       <c r="H48" s="8"/>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
@@ -10332,13 +10580,13 @@
       <c r="L48" s="5"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="39"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="35"/>
+      <c r="A49" s="44"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="41"/>
       <c r="H49" s="8"/>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
@@ -10346,13 +10594,13 @@
       <c r="L49" s="5"/>
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="39"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="35"/>
+      <c r="A50" s="44"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="41"/>
       <c r="H50" s="8"/>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
@@ -10360,13 +10608,13 @@
       <c r="L50" s="5"/>
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="39"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="35"/>
+      <c r="A51" s="44"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="41"/>
       <c r="H51" s="8"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
@@ -10374,13 +10622,13 @@
       <c r="L51" s="5"/>
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="39"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="35"/>
+      <c r="A52" s="44"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="41"/>
       <c r="H52" s="8"/>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
@@ -10388,13 +10636,13 @@
       <c r="L52" s="5"/>
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="39"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="35"/>
+      <c r="A53" s="44"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="41"/>
       <c r="H53" s="8"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
@@ -10402,13 +10650,13 @@
       <c r="L53" s="5"/>
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="39"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="35"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="41"/>
       <c r="H54" s="8"/>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
@@ -10416,13 +10664,13 @@
       <c r="L54" s="5"/>
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="39"/>
-      <c r="B55" s="34"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="35"/>
+      <c r="A55" s="44"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="41"/>
       <c r="H55" s="8"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
@@ -10430,13 +10678,13 @@
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="39"/>
-      <c r="B56" s="34"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="35"/>
+      <c r="A56" s="44"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="41"/>
       <c r="H56" s="8"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
@@ -10444,13 +10692,13 @@
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="39"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="35"/>
+      <c r="A57" s="44"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="41"/>
       <c r="H57" s="8"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
@@ -10458,13 +10706,13 @@
       <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="39"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="35"/>
+      <c r="A58" s="44"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="41"/>
       <c r="H58" s="8"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
@@ -10472,13 +10720,13 @@
       <c r="L58" s="5"/>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="39"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="35"/>
+      <c r="A59" s="44"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="41"/>
       <c r="H59" s="8"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
@@ -10486,13 +10734,13 @@
       <c r="L59" s="5"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="39"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="35"/>
+      <c r="A60" s="44"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="41"/>
       <c r="H60" s="8"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
@@ -10500,13 +10748,13 @@
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="39"/>
-      <c r="B61" s="34"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="35"/>
+      <c r="A61" s="44"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="41"/>
       <c r="H61" s="8"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
@@ -10514,13 +10762,13 @@
       <c r="L61" s="5"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="39"/>
-      <c r="B62" s="34"/>
-      <c r="C62" s="34"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="35"/>
+      <c r="A62" s="44"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="41"/>
       <c r="H62" s="8"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
@@ -10528,13 +10776,13 @@
       <c r="L62" s="5"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="39"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="35"/>
+      <c r="A63" s="44"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="41"/>
       <c r="H63" s="8"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
@@ -10542,13 +10790,13 @@
       <c r="L63" s="5"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="39"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="35"/>
+      <c r="A64" s="44"/>
+      <c r="B64" s="40"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="41"/>
       <c r="H64" s="8"/>
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
@@ -10556,13 +10804,13 @@
       <c r="L64" s="5"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="39"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="35"/>
+      <c r="A65" s="44"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="41"/>
       <c r="H65" s="8"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
@@ -10570,13 +10818,13 @@
       <c r="L65" s="5"/>
     </row>
     <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="39"/>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="35"/>
+      <c r="A66" s="44"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="41"/>
       <c r="H66" s="8"/>
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
@@ -10584,13 +10832,13 @@
       <c r="L66" s="5"/>
     </row>
     <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="39"/>
-      <c r="B67" s="34"/>
-      <c r="C67" s="34"/>
-      <c r="D67" s="34"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="35"/>
+      <c r="A67" s="44"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="40"/>
+      <c r="G67" s="41"/>
       <c r="H67" s="8"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
@@ -13862,7 +14110,7 @@
       </c>
       <c r="E1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45392</v>
+        <v>45417</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14338,30 +14586,30 @@
       <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="35"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="41"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="35"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="6" t="s">
         <v>10</v>
       </c>
@@ -14377,13 +14625,13 @@
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
       <c r="H29" s="22"/>
       <c r="I29" s="7"/>
       <c r="J29" s="16"/>
@@ -14392,13 +14640,13 @@
       <c r="N29" s="9"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="39"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
+      <c r="A30" s="44"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="41"/>
       <c r="H30" s="22"/>
       <c r="I30" s="7"/>
       <c r="J30" s="11"/>
@@ -14407,13 +14655,13 @@
       <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="39"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="35"/>
+      <c r="A31" s="44"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="41"/>
       <c r="H31" s="22"/>
       <c r="I31" s="7"/>
       <c r="J31" s="18"/>
@@ -14421,13 +14669,13 @@
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="39"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
+      <c r="A32" s="44"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="41"/>
       <c r="H32" s="22"/>
       <c r="I32" s="7"/>
       <c r="J32" s="11"/>
@@ -14435,13 +14683,13 @@
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="46"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="41"/>
       <c r="H33" s="22"/>
       <c r="I33" s="20"/>
       <c r="J33" s="25"/>
@@ -14449,13 +14697,13 @@
       <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="47"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="45"/>
+      <c r="A34" s="53"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="50"/>
       <c r="H34" s="27"/>
       <c r="I34" s="28"/>
       <c r="J34" s="30"/>
@@ -14463,13 +14711,13 @@
       <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="47"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="45"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="50"/>
       <c r="H35" s="27"/>
       <c r="I35" s="28"/>
       <c r="J35" s="30"/>
@@ -14477,13 +14725,13 @@
       <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="47"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="45"/>
+      <c r="A36" s="53"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="50"/>
       <c r="H36" s="27"/>
       <c r="I36" s="28"/>
       <c r="J36" s="30"/>
@@ -14491,13 +14739,13 @@
       <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="47"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="45"/>
+      <c r="A37" s="53"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="50"/>
       <c r="H37" s="27"/>
       <c r="I37" s="28"/>
       <c r="J37" s="30"/>
@@ -14505,13 +14753,13 @@
       <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="47"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="45"/>
+      <c r="A38" s="53"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="50"/>
       <c r="H38" s="27"/>
       <c r="I38" s="28"/>
       <c r="J38" s="30"/>
@@ -14519,13 +14767,13 @@
       <c r="L38" s="5"/>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="47"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="45"/>
+      <c r="A39" s="53"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="50"/>
       <c r="H39" s="27"/>
       <c r="I39" s="28"/>
       <c r="J39" s="30"/>
@@ -14533,13 +14781,13 @@
       <c r="L39" s="5"/>
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="47"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="45"/>
+      <c r="A40" s="53"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="50"/>
       <c r="H40" s="27"/>
       <c r="I40" s="28"/>
       <c r="J40" s="30"/>
@@ -14547,13 +14795,13 @@
       <c r="L40" s="5"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="47"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="45"/>
+      <c r="A41" s="53"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="50"/>
       <c r="H41" s="27"/>
       <c r="I41" s="28"/>
       <c r="J41" s="30"/>
@@ -14561,13 +14809,13 @@
       <c r="L41" s="5"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="47"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="45"/>
+      <c r="A42" s="53"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="50"/>
       <c r="H42" s="27"/>
       <c r="I42" s="28"/>
       <c r="J42" s="30"/>
@@ -14575,13 +14823,13 @@
       <c r="L42" s="5"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="47"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="45"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="50"/>
       <c r="H43" s="31"/>
       <c r="I43" s="28"/>
       <c r="J43" s="28"/>
@@ -14589,13 +14837,13 @@
       <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="47"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="50"/>
       <c r="H44" s="27"/>
       <c r="I44" s="28"/>
       <c r="J44" s="28"/>
@@ -14603,13 +14851,13 @@
       <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="39"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="35"/>
+      <c r="A45" s="44"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="41"/>
       <c r="H45" s="22"/>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
@@ -14617,13 +14865,13 @@
       <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="39"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="35"/>
+      <c r="A46" s="44"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="41"/>
       <c r="H46" s="8"/>
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
@@ -14631,13 +14879,13 @@
       <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="39"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="35"/>
+      <c r="A47" s="44"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="41"/>
       <c r="H47" s="8"/>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
@@ -14645,13 +14893,13 @@
       <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="39"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="35"/>
+      <c r="A48" s="44"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="41"/>
       <c r="H48" s="8"/>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
@@ -14659,13 +14907,13 @@
       <c r="L48" s="5"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="39"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="35"/>
+      <c r="A49" s="44"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="41"/>
       <c r="H49" s="8"/>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
@@ -14673,13 +14921,13 @@
       <c r="L49" s="5"/>
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="39"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="35"/>
+      <c r="A50" s="44"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="41"/>
       <c r="H50" s="8"/>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
@@ -14687,13 +14935,13 @@
       <c r="L50" s="5"/>
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="39"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="35"/>
+      <c r="A51" s="44"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="41"/>
       <c r="H51" s="8"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
@@ -14701,13 +14949,13 @@
       <c r="L51" s="5"/>
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="39"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="35"/>
+      <c r="A52" s="44"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="41"/>
       <c r="H52" s="8"/>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
@@ -14715,13 +14963,13 @@
       <c r="L52" s="5"/>
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="39"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="35"/>
+      <c r="A53" s="44"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="41"/>
       <c r="H53" s="8"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
@@ -14729,13 +14977,13 @@
       <c r="L53" s="5"/>
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="39"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="35"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="41"/>
       <c r="H54" s="8"/>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
@@ -14743,13 +14991,13 @@
       <c r="L54" s="5"/>
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="39"/>
-      <c r="B55" s="34"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="35"/>
+      <c r="A55" s="44"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="41"/>
       <c r="H55" s="8"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
@@ -14757,13 +15005,13 @@
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="39"/>
-      <c r="B56" s="34"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="35"/>
+      <c r="A56" s="44"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="41"/>
       <c r="H56" s="8"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
@@ -14771,13 +15019,13 @@
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="39"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="35"/>
+      <c r="A57" s="44"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="41"/>
       <c r="H57" s="8"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
@@ -14785,13 +15033,13 @@
       <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="39"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="35"/>
+      <c r="A58" s="44"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="41"/>
       <c r="H58" s="8"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
@@ -14799,13 +15047,13 @@
       <c r="L58" s="5"/>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="39"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="35"/>
+      <c r="A59" s="44"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="41"/>
       <c r="H59" s="8"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
@@ -14813,13 +15061,13 @@
       <c r="L59" s="5"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="39"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="35"/>
+      <c r="A60" s="44"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="41"/>
       <c r="H60" s="8"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
@@ -14827,13 +15075,13 @@
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="39"/>
-      <c r="B61" s="34"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="35"/>
+      <c r="A61" s="44"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="41"/>
       <c r="H61" s="8"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
@@ -14841,13 +15089,13 @@
       <c r="L61" s="5"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="39"/>
-      <c r="B62" s="34"/>
-      <c r="C62" s="34"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="35"/>
+      <c r="A62" s="44"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="41"/>
       <c r="H62" s="8"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
@@ -14855,13 +15103,13 @@
       <c r="L62" s="5"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="39"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="35"/>
+      <c r="A63" s="44"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="41"/>
       <c r="H63" s="8"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
@@ -14869,13 +15117,13 @@
       <c r="L63" s="5"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="39"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="35"/>
+      <c r="A64" s="44"/>
+      <c r="B64" s="40"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="41"/>
       <c r="H64" s="8"/>
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
@@ -14883,13 +15131,13 @@
       <c r="L64" s="5"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="39"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="35"/>
+      <c r="A65" s="44"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="41"/>
       <c r="H65" s="8"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
@@ -14897,13 +15145,13 @@
       <c r="L65" s="5"/>
     </row>
     <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="39"/>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="35"/>
+      <c r="A66" s="44"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="41"/>
       <c r="H66" s="8"/>
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
@@ -14911,13 +15159,13 @@
       <c r="L66" s="5"/>
     </row>
     <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="39"/>
-      <c r="B67" s="34"/>
-      <c r="C67" s="34"/>
-      <c r="D67" s="34"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="35"/>
+      <c r="A67" s="44"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="40"/>
+      <c r="G67" s="41"/>
       <c r="H67" s="8"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>

</xml_diff>